<commit_message>
Control and correction to inspo blocks
All the inspo blocks are now fully operational. The links and link names however still have to be checked
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lpe1b3v/Documents/Github/MailingTemplate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F082E5B-7EEB-264E-A426-34629F6A2E0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8863812F-00AF-6C4C-8A7B-AC34DB666A67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15940" xr2:uid="{C687F547-6D05-884E-B378-5AE1BA7C0F78}"/>
+    <workbookView xWindow="-28800" yWindow="5260" windowWidth="28800" windowHeight="17540" xr2:uid="{C687F547-6D05-884E-B378-5AE1BA7C0F78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,5 +538,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>